<commit_message>
Added correlation between defenders, modified excel defenders 2020
</commit_message>
<xml_diff>
--- a/difensori_2020.xlsx
+++ b/difensori_2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milan\OneDrive\Documenti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milan\OneDrive\Desktop\git shared\Pytone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4103197-9A51-4BD5-A403-56763C017DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C175CB-D832-45CD-BE19-D0255C2734EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{400D4252-A0EF-405E-A42D-DDEB3E8C3981}"/>
   </bookViews>
@@ -3262,7 +3262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3336,8 +3336,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3676,8 +3679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6065CA-7E41-4677-AEB8-D4CB7403B036}">
   <dimension ref="A1:BU229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BT2" sqref="BT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4120,6 +4123,9 @@
       </c>
       <c r="BS2" s="9" t="s">
         <v>80</v>
+      </c>
+      <c r="BT2" s="26">
+        <v>6</v>
       </c>
       <c r="BU2">
         <f>SUM(BQ2)+(BR2)</f>

</xml_diff>